<commit_message>
moved vs stuff -> vectorstore
</commit_message>
<xml_diff>
--- a/chroma-combos.xlsx
+++ b/chroma-combos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\8fort\dev\kfchat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB08A6D6-A857-47CE-9C11-1BB04CBB08BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EA5C952-FE30-4889-B6F1-9D7337D487BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-16290" yWindow="6765" windowWidth="16170" windowHeight="16860" xr2:uid="{FE525A8B-67A9-4D22-A197-2B0D31E7EB15}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="28">
   <si>
     <t>name</t>
   </si>
@@ -71,15 +71,6 @@
     <t>t3small</t>
   </si>
   <si>
-    <t>nomic</t>
-  </si>
-  <si>
-    <t>snowflake</t>
-  </si>
-  <si>
-    <t>mxbai</t>
-  </si>
-  <si>
     <t>granite</t>
   </si>
   <si>
@@ -104,26 +95,38 @@
     <t>Spacy</t>
   </si>
   <si>
-    <t>minilml6</t>
-  </si>
-  <si>
-    <t>mpnetbase</t>
-  </si>
-  <si>
     <t>Y</t>
   </si>
   <si>
+    <t>N</t>
+  </si>
+  <si>
     <t>*</t>
   </si>
   <si>
     <t>kfalcami 2025-02-15</t>
+  </si>
+  <si>
+    <t>[ERROR] [chromadbpage:handle_upload] [...] Error ingesting oregon.pdf: Error adding embeddings to o-granite-sc function:OllamaEmbeddingFunction type:Ollama-Embeddings: timed out in add. (is model loaded in ollama?)</t>
+  </si>
+  <si>
+    <t>nomic-embed-text,snowflake-arctic-embed2,mxbai-embed-large,granite-embedding:278m</t>
+  </si>
+  <si>
+    <t>[WARNING] [vschroma:ingest] [...] Error adding embeddings to gh-t3large-all function:OpenAIEmbeddingFunction type:Github-OpenAI-Embeddings: APIStatusError.__init__() missing 2 required keyword-only arguments: 'response' and 'body'</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>all-MiniLM-L6-v2,all-mpnet-base-v2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -146,6 +149,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -155,7 +174,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -215,11 +234,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -240,6 +270,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -589,10 +622,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92C505A6-2354-4712-8289-951E1069F707}">
-  <dimension ref="A1:G29"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+      <selection activeCell="A7" sqref="A7:XFD10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -601,11 +634,12 @@
     <col min="3" max="3" width="11.21875" style="5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.88671875" style="5"/>
     <col min="5" max="6" width="8.88671875" style="6"/>
+    <col min="7" max="7" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B1" s="8"/>
       <c r="C1" s="8"/>
@@ -624,270 +658,260 @@
         <v>2</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>16</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="G2" s="12"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B3" s="5" t="s">
         <v>3</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>24</v>
+        <v>19</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D4" s="5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D5" s="5" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D6" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B7" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E6" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C7" s="5" t="s">
-        <v>23</v>
-      </c>
       <c r="D7" s="5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D8" s="5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D9" s="5" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D10" s="5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B11" s="5" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D12" s="5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="G12" s="2"/>
+        <v>19</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D13" s="5" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D14" s="5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B15" s="5" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="F15" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="G15" s="10" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D16" s="5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="G16" s="2"/>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
       <c r="D17" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="D18" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="C19" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B20" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="C21" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F21" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E17" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="F17" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="D18" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E18" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="F18" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B19" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="D20" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="D21" s="5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="D22" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C24" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C25" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C26" s="5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B27" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C28" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C29" s="5" t="s">
+      <c r="G21" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="C22" s="5" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>